<commit_message>
Adding the extent report changes
</commit_message>
<xml_diff>
--- a/SVCareers_Automation_Testing_Project/Data/AddToRequisition.xlsx
+++ b/SVCareers_Automation_Testing_Project/Data/AddToRequisition.xlsx
@@ -32,9 +32,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>shashi.srinivas</t>
-  </si>
-  <si>
     <t>sv123</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>Manjunath Jayaram</t>
+  </si>
+  <si>
+    <t>supreeth.b</t>
   </si>
 </sst>
 </file>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,72 +479,72 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>29</v>
-      </c>
-      <c r="T1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -553,16 +553,16 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -571,22 +571,22 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>32</v>
-      </c>
-      <c r="T2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the delay wwhile executing scripts
</commit_message>
<xml_diff>
--- a/SVCareers_Automation_Testing_Project/Data/AddToRequisition.xlsx
+++ b/SVCareers_Automation_Testing_Project/Data/AddToRequisition.xlsx
@@ -32,6 +32,9 @@
     <t>Password</t>
   </si>
   <si>
+    <t>shashi.srinivas</t>
+  </si>
+  <si>
     <t>sv123</t>
   </si>
   <si>
@@ -123,16 +126,13 @@
   </si>
   <si>
     <t>Manjunath Jayaram</t>
-  </si>
-  <si>
-    <t>supreeth.b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,16 +140,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -157,12 +171,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +477,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,124 +503,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" t="s">
+      <c r="R1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" t="s">
+      <c r="S1" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>100</v>
+      </c>
+      <c r="F2" s="2">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
+      <formula1>"High,Medium,Low"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3">
+      <formula1>"NO,YES"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
+      <formula1>"Regular,Pipeline,RFP"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M3">
+      <formula1>"Replacement,New Position"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
+      <formula1>"Supreeth B,Adnim spiProject"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2">
+      <formula1>"Supreeth B,Adnim spiProject,Alex D Parker"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P7 Q2:Q6 R2 S2">
+      <formula1>"Client,Hiring Manager,HR,Other,Technical,Written"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>